<commit_message>
added mounting holes, added silk screen outlines, and vchanged LED resistor values
</commit_message>
<xml_diff>
--- a/Project Outputs for BMS_Masterboard (Trapezoid)/BOM/Bill of Materials-BMS_Masterboard (Trapezoid).xlsx
+++ b/Project Outputs for BMS_Masterboard (Trapezoid)/BOM/Bill of Materials-BMS_Masterboard (Trapezoid).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bseri\Desktop\Formula Material\MasterBoardGit\MasterBoard (Trapezoid)\Project Outputs for BMS_Masterboard (Trapezoid)\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B89EB08C-9680-4443-ADC3-ABCC05B0ED30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC346B5B-788D-4E41-970E-AB8CC06CB211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{F9B6ABE5-D4D9-43E1-A021-E14B9B7BE0E1}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" xr2:uid="{95539EA6-3DDB-4837-949F-D9D673B9B0A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BMS_Masterboa" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
   <si>
     <t>Quantity</t>
   </si>
@@ -169,6 +169,9 @@
     <t>No Description Available</t>
   </si>
   <si>
+    <t>R7</t>
+  </si>
+  <si>
     <t>R21</t>
   </si>
   <si>
@@ -367,12 +370,21 @@
     <t>R30, R32</t>
   </si>
   <si>
-    <t xml:space="preserve"> 27W4914</t>
+    <t>27W4914</t>
   </si>
   <si>
     <t>RES Thick Film, 300Ω, 1%, 0.25W, 100ppm/°C, 1206</t>
   </si>
   <si>
+    <t>R33, R35</t>
+  </si>
+  <si>
+    <t>P160ADCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 160 OHM 5% 1/2W 0805</t>
+  </si>
+  <si>
     <t>R16, R17, R34</t>
   </si>
   <si>
@@ -394,6 +406,9 @@
     <t>490-6060-1-ND</t>
   </si>
   <si>
+    <t>R1, R2, R3, R4, R5, R6</t>
+  </si>
+  <si>
     <t>R19, R20, R22, R23, R24, R25</t>
   </si>
   <si>
@@ -407,15 +422,6 @@
   </si>
   <si>
     <t>490-5803-1-ND</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R33, R35</t>
-  </si>
-  <si>
-    <t>P160ADCT-ND, P16076CT-ND</t>
-  </si>
-  <si>
-    <t>RES SMD 160 OHM 5% 1/2W 0805, RES SMD 665 OHM 1% 1/2W 0805</t>
   </si>
   <si>
     <t>AIR Signal NMOS, AIR_OPEN_SIGNAL, CANH, CANL, CHANNEL1, CHANNEL2, Charging Signal, Charging Signal NMOS, TP_CS, TP_MISO, TP_MOSI, TP_SCK, VCC_3.3V, VCC_5V</t>
@@ -797,8 +803,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93CE1F1-FC3D-438A-A1A8-9F1555F1912A}">
-  <dimension ref="A1:E49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4528F2-EE65-4C01-ACAF-45207E540145}">
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1107,12 +1113,8 @@
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1122,13 +1124,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
@@ -1142,13 +1144,13 @@
         <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1156,16 +1158,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1173,16 +1175,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1190,16 +1192,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1207,16 +1209,16 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1224,16 +1226,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1241,16 +1243,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1258,16 +1260,16 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1275,16 +1277,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1292,33 +1294,33 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1326,16 +1328,16 @@
         <v>2</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1343,16 +1345,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1360,16 +1362,16 @@
         <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1377,16 +1379,16 @@
         <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1394,16 +1396,16 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1411,16 +1413,16 @@
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1428,16 +1430,16 @@
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1445,16 +1447,16 @@
         <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1462,16 +1464,16 @@
         <v>2</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1479,16 +1481,16 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1496,16 +1498,16 @@
         <v>2</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1513,98 +1515,98 @@
         <v>2</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E42" s="2" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>17</v>
@@ -1612,32 +1614,62 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>124</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
+        <v>6</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>8</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
         <v>14</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="2" t="s">
-        <v>127</v>
+      <c r="B51" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>